<commit_message>
Streamline various elements and element headings
</commit_message>
<xml_diff>
--- a/DCC_template.xlsx
+++ b/DCC_template.xlsx
@@ -1,43 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tesla\Data\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C7BF0A-F1BA-45F5-8A64-7875F2D555E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8BAE9A5-058C-430A-8E32-91B299938AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="34320" windowHeight="19680" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="885" yWindow="2025" windowWidth="37200" windowHeight="17310" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="10" state="hidden" r:id="rId1"/>
     <sheet name="statements" sheetId="5" r:id="rId2"/>
-    <sheet name="Table" sheetId="11" r:id="rId3"/>
+    <sheet name="AdministrativeData" sheetId="12" r:id="rId3"/>
+    <sheet name="Table" sheetId="11" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="ColType" localSheetId="0">Definitions!$A$2:$A$7</definedName>
-    <definedName name="ColType" localSheetId="2">Definitions!$A$2:$A$7</definedName>
+    <definedName name="ColType" localSheetId="3">Definitions!$A$2:$A$7</definedName>
     <definedName name="ColType">[1]Definitions!$A$2:$A$7</definedName>
     <definedName name="EquipmentCategories">Definitions!$G$2:$G$3</definedName>
     <definedName name="MeasurandType" localSheetId="0">Definitions!$C$2:$C$153</definedName>
-    <definedName name="MeasurandType" localSheetId="2">Definitions!$C$2:$C$153</definedName>
+    <definedName name="MeasurandType" localSheetId="3">Definitions!$C$2:$C$153</definedName>
     <definedName name="MeasurandType">[1]Definitions!$C$2:$C$153</definedName>
     <definedName name="metaDataType" localSheetId="0">Definitions!$I$2:$I$11</definedName>
-    <definedName name="metaDataType" localSheetId="2">Definitions!$I$2:$I$11</definedName>
+    <definedName name="metaDataType" localSheetId="3">Definitions!$I$2:$I$11</definedName>
     <definedName name="metaDataType">[1]Definitions!$I$2:$I$11</definedName>
     <definedName name="MetaType" localSheetId="0">Definitions!$B$2:$B$21</definedName>
-    <definedName name="MetaType" localSheetId="2">Definitions!$B$2:$B$21</definedName>
+    <definedName name="MetaType" localSheetId="3">Definitions!$B$2:$B$21</definedName>
     <definedName name="MetaType">[1]Definitions!$B$2:$B$21</definedName>
     <definedName name="rgKommentar">[2]ODBC!$O$7:$P$19</definedName>
     <definedName name="statementCategories">Definitions!$F$2:$F$10</definedName>
-    <definedName name="UsedReference" localSheetId="2">Table!metaDataType</definedName>
+    <definedName name="UsedReference" localSheetId="3">Table!metaDataType</definedName>
     <definedName name="UsedReference">Definitions!metaDataType</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -862,7 +863,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -926,6 +927,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCE4D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1008,7 +1021,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1098,6 +1111,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3814,10 +3836,236 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ACB4920-6201-4376-ABCA-989A89C97750}">
+  <dimension ref="A1:O49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="67.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="32"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="33"/>
+      <c r="B20" s="33"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="33"/>
+      <c r="B26" s="33"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="34"/>
+      <c r="B35" s="34"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="30"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="30"/>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="30"/>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="30"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1CAB232-3A04-4E0E-965E-F5ECA0CF44DC}">
   <dimension ref="A1:AC42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Change item to measuringInstrument
</commit_message>
<xml_diff>
--- a/DCC_template.xlsx
+++ b/DCC_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tesla\Data\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC6F898-D1EC-408C-A34F-B2ED3BEB6160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37B47B7-1959-4827-A85A-6220CA80B02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="3015" windowWidth="28800" windowHeight="15555" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="1020" windowWidth="34680" windowHeight="14385" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="10" state="hidden" r:id="rId1"/>
@@ -22,10 +22,12 @@
     <sheet name="Table4" sheetId="16" r:id="rId7"/>
     <sheet name="Table5" sheetId="14" r:id="rId8"/>
     <sheet name="Table6" sheetId="11" r:id="rId9"/>
+    <sheet name="Table7" sheetId="18" r:id="rId10"/>
+    <sheet name="Table8" sheetId="19" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
-    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
     <definedName name="ColType" localSheetId="0">Definitions!$A$2:$A$7</definedName>
@@ -35,6 +37,8 @@
     <definedName name="ColType" localSheetId="6">Definitions!$A$2:$A$7</definedName>
     <definedName name="ColType" localSheetId="7">Definitions!$A$2:$A$7</definedName>
     <definedName name="ColType" localSheetId="8">Definitions!$A$2:$A$7</definedName>
+    <definedName name="ColType" localSheetId="9">Definitions!$A$2:$A$7</definedName>
+    <definedName name="ColType" localSheetId="10">Definitions!$A$2:$A$7</definedName>
     <definedName name="ColType">[1]Definitions!$A$2:$A$7</definedName>
     <definedName name="EquipmentCategories">Definitions!$G$2:$G$3</definedName>
     <definedName name="MeasurandType" localSheetId="0">Definitions!$C$2:$C$153</definedName>
@@ -44,6 +48,8 @@
     <definedName name="MeasurandType" localSheetId="6">Definitions!$C$2:$C$153</definedName>
     <definedName name="MeasurandType" localSheetId="7">Definitions!$C$2:$C$153</definedName>
     <definedName name="MeasurandType" localSheetId="8">Definitions!$C$2:$C$153</definedName>
+    <definedName name="MeasurandType" localSheetId="9">Definitions!$C$2:$C$153</definedName>
+    <definedName name="MeasurandType" localSheetId="10">Definitions!$C$2:$C$153</definedName>
     <definedName name="MeasurandType">[1]Definitions!$C$2:$C$153</definedName>
     <definedName name="metaDataType" localSheetId="0">Definitions!$I$2:$I$11</definedName>
     <definedName name="metaDataType" localSheetId="3">Definitions!$I$2:$I$11</definedName>
@@ -52,6 +58,8 @@
     <definedName name="metaDataType" localSheetId="6">Definitions!$I$2:$I$11</definedName>
     <definedName name="metaDataType" localSheetId="7">Definitions!$I$2:$I$11</definedName>
     <definedName name="metaDataType" localSheetId="8">Definitions!$I$2:$I$11</definedName>
+    <definedName name="metaDataType" localSheetId="9">Definitions!$I$2:$I$11</definedName>
+    <definedName name="metaDataType" localSheetId="10">Definitions!$I$2:$I$11</definedName>
     <definedName name="metaDataType">[1]Definitions!$I$2:$I$11</definedName>
     <definedName name="MetaType" localSheetId="0">Definitions!$B$2:$B$21</definedName>
     <definedName name="MetaType" localSheetId="3">Definitions!$B$2:$B$21</definedName>
@@ -60,6 +68,8 @@
     <definedName name="MetaType" localSheetId="6">Definitions!$B$2:$B$21</definedName>
     <definedName name="MetaType" localSheetId="7">Definitions!$B$2:$B$21</definedName>
     <definedName name="MetaType" localSheetId="8">Definitions!$B$2:$B$21</definedName>
+    <definedName name="MetaType" localSheetId="9">Definitions!$B$2:$B$21</definedName>
+    <definedName name="MetaType" localSheetId="10">Definitions!$B$2:$B$21</definedName>
     <definedName name="MetaType">[1]Definitions!$B$2:$B$21</definedName>
     <definedName name="rgKommentar">[2]ODBC!$O$7:$P$19</definedName>
     <definedName name="statementCategories">Definitions!$F$2:$F$10</definedName>
@@ -69,6 +79,8 @@
     <definedName name="UsedReference" localSheetId="6">Table4!metaDataType</definedName>
     <definedName name="UsedReference" localSheetId="7">Table5!metaDataType</definedName>
     <definedName name="UsedReference" localSheetId="8">Table6!metaDataType</definedName>
+    <definedName name="UsedReference" localSheetId="9">Table7!metaDataType</definedName>
+    <definedName name="UsedReference" localSheetId="10">Table8!metaDataType</definedName>
     <definedName name="UsedReference">Definitions!metaDataType</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -3627,6 +3639,2284 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE98357-5008-41F4-A1D2-85A610305A8A}">
+  <dimension ref="A1:AC42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A18" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+    </row>
+    <row r="2" spans="1:29" ht="17.25" customHeight="1">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+    </row>
+    <row r="5" spans="1:29">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+    </row>
+    <row r="6" spans="1:29">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:29">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:29">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:29">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+    </row>
+    <row r="10" spans="1:29">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+    </row>
+    <row r="12" spans="1:29">
+      <c r="A12" s="28"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+    </row>
+    <row r="13" spans="1:29">
+      <c r="A13" s="26"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+    </row>
+    <row r="14" spans="1:29">
+      <c r="A14" s="24"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="24"/>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="24"/>
+      <c r="AB14" s="24"/>
+      <c r="AC14" s="24"/>
+    </row>
+    <row r="15" spans="1:29">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="10"/>
+    </row>
+    <row r="16" spans="1:29">
+      <c r="A16" s="13"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
+      <c r="AC16" s="10"/>
+    </row>
+    <row r="17" spans="1:29">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
+    </row>
+    <row r="18" spans="1:29">
+      <c r="A18" s="13"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="10"/>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="10"/>
+    </row>
+    <row r="19" spans="1:29">
+      <c r="A19" s="6"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="10"/>
+    </row>
+    <row r="20" spans="1:29">
+      <c r="A20" s="6"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="10"/>
+    </row>
+    <row r="21" spans="1:29">
+      <c r="A21" s="6"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="10"/>
+    </row>
+    <row r="22" spans="1:29">
+      <c r="A22" s="6"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
+    </row>
+    <row r="23" spans="1:29">
+      <c r="A23" s="6"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="10"/>
+      <c r="AB23" s="10"/>
+      <c r="AC23" s="10"/>
+    </row>
+    <row r="24" spans="1:29">
+      <c r="A24" s="6"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="10"/>
+      <c r="AA24" s="10"/>
+      <c r="AB24" s="10"/>
+      <c r="AC24" s="10"/>
+    </row>
+    <row r="25" spans="1:29">
+      <c r="A25" s="6"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="10"/>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="10"/>
+    </row>
+    <row r="26" spans="1:29">
+      <c r="A26" s="6"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10"/>
+      <c r="AA26" s="10"/>
+      <c r="AB26" s="10"/>
+      <c r="AC26" s="10"/>
+    </row>
+    <row r="27" spans="1:29">
+      <c r="A27" s="6"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="10"/>
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="10"/>
+    </row>
+    <row r="28" spans="1:29">
+      <c r="A28" s="6"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="10"/>
+      <c r="X28" s="10"/>
+      <c r="Y28" s="10"/>
+      <c r="Z28" s="10"/>
+      <c r="AA28" s="10"/>
+      <c r="AB28" s="10"/>
+      <c r="AC28" s="10"/>
+    </row>
+    <row r="29" spans="1:29">
+      <c r="A29" s="6"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+      <c r="W29" s="10"/>
+      <c r="X29" s="10"/>
+      <c r="Y29" s="10"/>
+      <c r="Z29" s="10"/>
+      <c r="AA29" s="10"/>
+      <c r="AB29" s="10"/>
+      <c r="AC29" s="10"/>
+    </row>
+    <row r="30" spans="1:29">
+      <c r="A30" s="6"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="10"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="10"/>
+      <c r="AB30" s="10"/>
+      <c r="AC30" s="10"/>
+    </row>
+    <row r="31" spans="1:29">
+      <c r="A31" s="6"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10"/>
+      <c r="X31" s="10"/>
+      <c r="Y31" s="10"/>
+      <c r="Z31" s="10"/>
+      <c r="AA31" s="10"/>
+      <c r="AB31" s="10"/>
+      <c r="AC31" s="10"/>
+    </row>
+    <row r="32" spans="1:29">
+      <c r="A32" s="6"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10"/>
+      <c r="V32" s="10"/>
+      <c r="W32" s="10"/>
+      <c r="X32" s="10"/>
+      <c r="Y32" s="10"/>
+      <c r="Z32" s="10"/>
+      <c r="AA32" s="10"/>
+      <c r="AB32" s="10"/>
+      <c r="AC32" s="10"/>
+    </row>
+    <row r="33" spans="1:29">
+      <c r="A33" s="6"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
+      <c r="W33" s="10"/>
+      <c r="X33" s="10"/>
+      <c r="Y33" s="10"/>
+      <c r="Z33" s="10"/>
+      <c r="AA33" s="10"/>
+      <c r="AB33" s="10"/>
+      <c r="AC33" s="10"/>
+    </row>
+    <row r="34" spans="1:29">
+      <c r="A34" s="6"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="10"/>
+      <c r="Y34" s="10"/>
+      <c r="Z34" s="10"/>
+      <c r="AA34" s="10"/>
+      <c r="AB34" s="10"/>
+      <c r="AC34" s="10"/>
+    </row>
+    <row r="35" spans="1:29">
+      <c r="A35" s="6"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
+      <c r="W35" s="10"/>
+      <c r="X35" s="10"/>
+      <c r="Y35" s="10"/>
+      <c r="Z35" s="10"/>
+      <c r="AA35" s="10"/>
+      <c r="AB35" s="10"/>
+      <c r="AC35" s="10"/>
+    </row>
+    <row r="36" spans="1:29">
+      <c r="A36" s="6"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+      <c r="T36" s="10"/>
+      <c r="U36" s="10"/>
+      <c r="V36" s="10"/>
+      <c r="W36" s="10"/>
+      <c r="X36" s="10"/>
+      <c r="Y36" s="10"/>
+      <c r="Z36" s="10"/>
+      <c r="AA36" s="10"/>
+      <c r="AB36" s="10"/>
+      <c r="AC36" s="10"/>
+    </row>
+    <row r="37" spans="1:29">
+      <c r="A37" s="6"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="10"/>
+      <c r="W37" s="10"/>
+      <c r="X37" s="10"/>
+      <c r="Y37" s="10"/>
+      <c r="Z37" s="10"/>
+      <c r="AA37" s="10"/>
+      <c r="AB37" s="10"/>
+      <c r="AC37" s="10"/>
+    </row>
+    <row r="38" spans="1:29">
+      <c r="A38" s="6"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10"/>
+      <c r="W38" s="10"/>
+      <c r="X38" s="10"/>
+      <c r="Y38" s="10"/>
+      <c r="Z38" s="10"/>
+      <c r="AA38" s="10"/>
+      <c r="AB38" s="10"/>
+      <c r="AC38" s="10"/>
+    </row>
+    <row r="39" spans="1:29">
+      <c r="A39" s="6"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="10"/>
+      <c r="W39" s="10"/>
+      <c r="X39" s="10"/>
+      <c r="Y39" s="10"/>
+      <c r="Z39" s="10"/>
+      <c r="AA39" s="10"/>
+      <c r="AB39" s="10"/>
+      <c r="AC39" s="10"/>
+    </row>
+    <row r="40" spans="1:29">
+      <c r="A40" s="6"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="10"/>
+      <c r="U40" s="10"/>
+      <c r="V40" s="10"/>
+      <c r="W40" s="10"/>
+      <c r="X40" s="10"/>
+      <c r="Y40" s="10"/>
+      <c r="Z40" s="10"/>
+      <c r="AA40" s="10"/>
+      <c r="AB40" s="10"/>
+      <c r="AC40" s="10"/>
+    </row>
+    <row r="41" spans="1:29">
+      <c r="A41" s="6"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
+      <c r="T41" s="10"/>
+      <c r="U41" s="10"/>
+      <c r="V41" s="10"/>
+      <c r="W41" s="10"/>
+      <c r="X41" s="10"/>
+      <c r="Y41" s="10"/>
+      <c r="Z41" s="10"/>
+      <c r="AA41" s="10"/>
+      <c r="AB41" s="10"/>
+      <c r="AC41" s="10"/>
+    </row>
+    <row r="42" spans="1:29">
+      <c r="A42" s="6"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
+      <c r="V42" s="10"/>
+      <c r="W42" s="10"/>
+      <c r="X42" s="10"/>
+      <c r="Y42" s="10"/>
+      <c r="Z42" s="10"/>
+      <c r="AA42" s="10"/>
+      <c r="AB42" s="10"/>
+      <c r="AC42" s="10"/>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <mergeCells count="1">
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:AC13" xr:uid="{E1CF1B6D-3795-4779-8280-DB4398D9899D}">
+      <formula1>metaDataType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:AC10" xr:uid="{39F0C12A-29CC-4A32-B83F-0A094253BEE8}">
+      <formula1>MetaType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:AC9" xr:uid="{24D96E29-1F30-480C-894D-74923BEE405E}">
+      <formula1>ColType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:AC11" xr:uid="{D27868AC-D066-443D-8618-1E6825521573}">
+      <formula1>MeasurandType</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA0930D-47C9-4C25-B7CD-6B5E90206B32}">
+  <dimension ref="A1:AC42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+    </row>
+    <row r="2" spans="1:29" ht="17.25" customHeight="1">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+    </row>
+    <row r="5" spans="1:29">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+    </row>
+    <row r="6" spans="1:29">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:29">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:29">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:29">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+    </row>
+    <row r="10" spans="1:29">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+    </row>
+    <row r="12" spans="1:29">
+      <c r="A12" s="28"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+    </row>
+    <row r="13" spans="1:29">
+      <c r="A13" s="26"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+    </row>
+    <row r="14" spans="1:29">
+      <c r="A14" s="24"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="24"/>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="24"/>
+      <c r="AB14" s="24"/>
+      <c r="AC14" s="24"/>
+    </row>
+    <row r="15" spans="1:29">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="10"/>
+    </row>
+    <row r="16" spans="1:29">
+      <c r="A16" s="13"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
+      <c r="AC16" s="10"/>
+    </row>
+    <row r="17" spans="1:29">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
+    </row>
+    <row r="18" spans="1:29">
+      <c r="A18" s="13"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="10"/>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="10"/>
+    </row>
+    <row r="19" spans="1:29">
+      <c r="A19" s="6"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="10"/>
+    </row>
+    <row r="20" spans="1:29">
+      <c r="A20" s="6"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="10"/>
+    </row>
+    <row r="21" spans="1:29">
+      <c r="A21" s="6"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="10"/>
+    </row>
+    <row r="22" spans="1:29">
+      <c r="A22" s="6"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
+    </row>
+    <row r="23" spans="1:29">
+      <c r="A23" s="6"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="10"/>
+      <c r="AB23" s="10"/>
+      <c r="AC23" s="10"/>
+    </row>
+    <row r="24" spans="1:29">
+      <c r="A24" s="6"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="10"/>
+      <c r="AA24" s="10"/>
+      <c r="AB24" s="10"/>
+      <c r="AC24" s="10"/>
+    </row>
+    <row r="25" spans="1:29">
+      <c r="A25" s="6"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="10"/>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="10"/>
+    </row>
+    <row r="26" spans="1:29">
+      <c r="A26" s="6"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10"/>
+      <c r="AA26" s="10"/>
+      <c r="AB26" s="10"/>
+      <c r="AC26" s="10"/>
+    </row>
+    <row r="27" spans="1:29">
+      <c r="A27" s="6"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="10"/>
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="10"/>
+    </row>
+    <row r="28" spans="1:29">
+      <c r="A28" s="6"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="10"/>
+      <c r="X28" s="10"/>
+      <c r="Y28" s="10"/>
+      <c r="Z28" s="10"/>
+      <c r="AA28" s="10"/>
+      <c r="AB28" s="10"/>
+      <c r="AC28" s="10"/>
+    </row>
+    <row r="29" spans="1:29">
+      <c r="A29" s="6"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+      <c r="W29" s="10"/>
+      <c r="X29" s="10"/>
+      <c r="Y29" s="10"/>
+      <c r="Z29" s="10"/>
+      <c r="AA29" s="10"/>
+      <c r="AB29" s="10"/>
+      <c r="AC29" s="10"/>
+    </row>
+    <row r="30" spans="1:29">
+      <c r="A30" s="6"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="10"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="10"/>
+      <c r="AB30" s="10"/>
+      <c r="AC30" s="10"/>
+    </row>
+    <row r="31" spans="1:29">
+      <c r="A31" s="6"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10"/>
+      <c r="X31" s="10"/>
+      <c r="Y31" s="10"/>
+      <c r="Z31" s="10"/>
+      <c r="AA31" s="10"/>
+      <c r="AB31" s="10"/>
+      <c r="AC31" s="10"/>
+    </row>
+    <row r="32" spans="1:29">
+      <c r="A32" s="6"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10"/>
+      <c r="V32" s="10"/>
+      <c r="W32" s="10"/>
+      <c r="X32" s="10"/>
+      <c r="Y32" s="10"/>
+      <c r="Z32" s="10"/>
+      <c r="AA32" s="10"/>
+      <c r="AB32" s="10"/>
+      <c r="AC32" s="10"/>
+    </row>
+    <row r="33" spans="1:29">
+      <c r="A33" s="6"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
+      <c r="W33" s="10"/>
+      <c r="X33" s="10"/>
+      <c r="Y33" s="10"/>
+      <c r="Z33" s="10"/>
+      <c r="AA33" s="10"/>
+      <c r="AB33" s="10"/>
+      <c r="AC33" s="10"/>
+    </row>
+    <row r="34" spans="1:29">
+      <c r="A34" s="6"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="10"/>
+      <c r="Y34" s="10"/>
+      <c r="Z34" s="10"/>
+      <c r="AA34" s="10"/>
+      <c r="AB34" s="10"/>
+      <c r="AC34" s="10"/>
+    </row>
+    <row r="35" spans="1:29">
+      <c r="A35" s="6"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
+      <c r="W35" s="10"/>
+      <c r="X35" s="10"/>
+      <c r="Y35" s="10"/>
+      <c r="Z35" s="10"/>
+      <c r="AA35" s="10"/>
+      <c r="AB35" s="10"/>
+      <c r="AC35" s="10"/>
+    </row>
+    <row r="36" spans="1:29">
+      <c r="A36" s="6"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+      <c r="T36" s="10"/>
+      <c r="U36" s="10"/>
+      <c r="V36" s="10"/>
+      <c r="W36" s="10"/>
+      <c r="X36" s="10"/>
+      <c r="Y36" s="10"/>
+      <c r="Z36" s="10"/>
+      <c r="AA36" s="10"/>
+      <c r="AB36" s="10"/>
+      <c r="AC36" s="10"/>
+    </row>
+    <row r="37" spans="1:29">
+      <c r="A37" s="6"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="10"/>
+      <c r="W37" s="10"/>
+      <c r="X37" s="10"/>
+      <c r="Y37" s="10"/>
+      <c r="Z37" s="10"/>
+      <c r="AA37" s="10"/>
+      <c r="AB37" s="10"/>
+      <c r="AC37" s="10"/>
+    </row>
+    <row r="38" spans="1:29">
+      <c r="A38" s="6"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10"/>
+      <c r="W38" s="10"/>
+      <c r="X38" s="10"/>
+      <c r="Y38" s="10"/>
+      <c r="Z38" s="10"/>
+      <c r="AA38" s="10"/>
+      <c r="AB38" s="10"/>
+      <c r="AC38" s="10"/>
+    </row>
+    <row r="39" spans="1:29">
+      <c r="A39" s="6"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="10"/>
+      <c r="W39" s="10"/>
+      <c r="X39" s="10"/>
+      <c r="Y39" s="10"/>
+      <c r="Z39" s="10"/>
+      <c r="AA39" s="10"/>
+      <c r="AB39" s="10"/>
+      <c r="AC39" s="10"/>
+    </row>
+    <row r="40" spans="1:29">
+      <c r="A40" s="6"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="10"/>
+      <c r="U40" s="10"/>
+      <c r="V40" s="10"/>
+      <c r="W40" s="10"/>
+      <c r="X40" s="10"/>
+      <c r="Y40" s="10"/>
+      <c r="Z40" s="10"/>
+      <c r="AA40" s="10"/>
+      <c r="AB40" s="10"/>
+      <c r="AC40" s="10"/>
+    </row>
+    <row r="41" spans="1:29">
+      <c r="A41" s="6"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
+      <c r="T41" s="10"/>
+      <c r="U41" s="10"/>
+      <c r="V41" s="10"/>
+      <c r="W41" s="10"/>
+      <c r="X41" s="10"/>
+      <c r="Y41" s="10"/>
+      <c r="Z41" s="10"/>
+      <c r="AA41" s="10"/>
+      <c r="AB41" s="10"/>
+      <c r="AC41" s="10"/>
+    </row>
+    <row r="42" spans="1:29">
+      <c r="A42" s="6"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
+      <c r="V42" s="10"/>
+      <c r="W42" s="10"/>
+      <c r="X42" s="10"/>
+      <c r="Y42" s="10"/>
+      <c r="Z42" s="10"/>
+      <c r="AA42" s="10"/>
+      <c r="AB42" s="10"/>
+      <c r="AC42" s="10"/>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <mergeCells count="1">
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:AC11" xr:uid="{002D8DE4-B068-4617-995C-1D6E7E65E991}">
+      <formula1>MeasurandType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:AC9" xr:uid="{C7880A94-D8B2-4439-8DAB-2818CF3F1962}">
+      <formula1>ColType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:AC10" xr:uid="{F675552D-35C2-45EF-9C5C-9F3CD1CDAACC}">
+      <formula1>MetaType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:AC13" xr:uid="{F7356F90-9F17-468A-A20F-447726D60A35}">
+      <formula1>metaDataType</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C1:E48"/>
@@ -9790,7 +12080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1CAB232-3A04-4E0E-965E-F5ECA0CF44DC}">
   <dimension ref="A1:AC42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>

</xml_diff>